<commit_message>
modified fiel of sendmail
</commit_message>
<xml_diff>
--- a/Email-SmS/duesRecords.xlsx
+++ b/Email-SmS/duesRecords.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\conding\py\autoprogram\Email-SmS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="120" windowWidth="12420" windowHeight="6360"/>
+    <workbookView xWindow="195" yWindow="120" windowWidth="12420" windowHeight="6360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="22">
   <si>
     <t>Member</t>
   </si>
@@ -43,21 +48,12 @@
     <t>Email</t>
   </si>
   <si>
-    <t>alice@example.com</t>
-  </si>
-  <si>
-    <t>bob@example.com</t>
-  </si>
-  <si>
     <t>carol@example.com</t>
   </si>
   <si>
     <t>david@example.com</t>
   </si>
   <si>
-    <t>eve@example.com</t>
-  </si>
-  <si>
     <t>fred@example.com</t>
   </si>
   <si>
@@ -77,17 +73,33 @@
   </si>
   <si>
     <t>paid</t>
+  </si>
+  <si>
+    <t>paid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXXX@sina.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXXXXXX@sina.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>xxxxxxx@163.com</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -95,7 +107,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -117,15 +144,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -133,12 +163,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -180,7 +213,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -215,7 +248,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -427,15 +460,15 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,146 +494,155 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>